<commit_message>
auto evaluvation and unique id for students
</commit_message>
<xml_diff>
--- a/lara-frontend/src/components/admin/Example_Paperbasedexcel_sheet.xlsx
+++ b/lara-frontend/src/components/admin/Example_Paperbasedexcel_sheet.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanne\OneDrive\Desktop\lara_grooming\lara-frontend\src\components\admin\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479782D6-1D33-4DC5-AC13-613406A04841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>obtainedMarks</t>
   </si>
   <si>
@@ -40,21 +31,9 @@
     <t>testName</t>
   </si>
   <si>
-    <t>abc@gmail.com</t>
-  </si>
-  <si>
-    <t>xyz@gmail.com</t>
-  </si>
-  <si>
-    <t>hello@gmail.com</t>
-  </si>
-  <si>
     <t>test1</t>
   </si>
   <si>
-    <t>rani@gmail.com</t>
-  </si>
-  <si>
     <t>core java</t>
   </si>
   <si>
@@ -67,25 +46,32 @@
     <t>test2</t>
   </si>
   <si>
-    <t>raja@gmail.com</t>
+    <t>studentId</t>
+  </si>
+  <si>
+    <t>JAV202500001</t>
+  </si>
+  <si>
+    <t>JAV202500002</t>
+  </si>
+  <si>
+    <t>JAV202500003</t>
+  </si>
+  <si>
+    <t>JAV202500004</t>
+  </si>
+  <si>
+    <t>JAV202500005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,17 +100,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,45 +447,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.09765625" customWidth="1"/>
-    <col min="3" max="3" width="11.09765625" customWidth="1"/>
-    <col min="4" max="4" width="13.19921875" customWidth="1"/>
-    <col min="5" max="5" width="14.19921875" customWidth="1"/>
-    <col min="6" max="6" width="9.796875" customWidth="1"/>
+    <col min="1" max="1" width="23.08203125" customWidth="1"/>
+    <col min="3" max="3" width="11.08203125" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B2">
         <v>80</v>
@@ -508,18 +494,18 @@
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="B3">
         <v>90</v>
@@ -528,18 +514,18 @@
         <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B4">
         <v>71</v>
@@ -548,18 +534,18 @@
         <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B5">
         <v>65</v>
@@ -568,17 +554,17 @@
         <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B6">
@@ -588,26 +574,19 @@
         <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{BA6FDE03-1D3B-4D88-8385-75E88F1FE12E}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{38229A76-3373-4315-9EF8-024CE4F47307}"/>
-    <hyperlink ref="A2" r:id="rId3" display="khema.cnp@gmail.com" xr:uid="{20DD9ACF-DBB0-4C9A-90C5-81330D2D8069}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{0D71F93D-7549-4B30-ABD6-FAE7B2631DD9}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{A49EC02F-5754-49C2-9600-465369B737FB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1 B3:C3 B2:C2" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:E1 B3:C3 B2:C2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>